<commit_message>
Save Load I2C config implemented
</commit_message>
<xml_diff>
--- a/EEPROM.xlsx
+++ b/EEPROM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Prog\Github\VCMC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85D336A-D6B2-4459-937E-39048C787380}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BF4F49-8F20-47F4-A1C5-BB088D79AD4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2570" yWindow="8160" windowWidth="24370" windowHeight="12590" xr2:uid="{70207959-F336-4C7B-99A5-F828907A22FB}"/>
+    <workbookView xWindow="16050" yWindow="740" windowWidth="19350" windowHeight="18390" xr2:uid="{70207959-F336-4C7B-99A5-F828907A22FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -444,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8FB32A5-7921-4AAC-8700-79D65AB1EF65}">
-  <dimension ref="A17:F37"/>
+  <dimension ref="A17:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -498,7 +498,7 @@
         <v>27</v>
       </c>
       <c r="D19">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F19">
         <f>38+5</f>
@@ -526,8 +526,7 @@
         <v>132</v>
       </c>
       <c r="D21">
-        <f>+D19+D18+D20</f>
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="F21">
         <f>+F19+F18+F20</f>
@@ -573,7 +572,7 @@
         <v>8</v>
       </c>
       <c r="D24">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F24">
         <v>8</v>
@@ -587,10 +586,10 @@
         <v>40</v>
       </c>
       <c r="C25">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D25">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F25">
         <v>24</v>
@@ -607,7 +606,7 @@
         <v>14</v>
       </c>
       <c r="D26">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -623,11 +622,11 @@
       </c>
       <c r="C27">
         <f>+C26+C25+C24+C23</f>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D27">
         <f>+D26+D25+D24+D23</f>
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F27">
         <f>+F26+F25+F24+F23</f>
@@ -661,11 +660,11 @@
       </c>
       <c r="C29">
         <f>+C28*C27+C25+C25+C24</f>
-        <v>390</v>
+        <v>400</v>
       </c>
       <c r="D29">
         <f>+D28*D27+D25+D25+D24</f>
-        <v>461</v>
+        <v>480</v>
       </c>
       <c r="F29">
         <f>+F28*F27+F25+F25+F24</f>
@@ -719,7 +718,7 @@
       </c>
       <c r="D33">
         <f>INT((D32-D21)/D29)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33">
         <f>INT((F32-F21)/F29)</f>
@@ -736,11 +735,11 @@
       </c>
       <c r="C34">
         <f>-C33*C29-C21+C32</f>
-        <v>356</v>
+        <v>316</v>
       </c>
       <c r="D34">
         <f>-D33*D29-D21+D32</f>
-        <v>72</v>
+        <v>458</v>
       </c>
       <c r="F34">
         <f>-F33*F29-F21+F32</f>
@@ -758,11 +757,17 @@
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C37">
         <f>+C29+150</f>
-        <v>540</v>
+        <v>550</v>
       </c>
       <c r="F37">
         <f>+F29+150</f>
         <v>478</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D38">
+        <f>+D32-D34</f>
+        <v>1590</v>
       </c>
     </row>
   </sheetData>

</xml_diff>